<commit_message>
Update profiles descriptions (#93) e50c5ba39214294e373398fdb69f87a0c54b73b5
</commit_message>
<xml_diff>
--- a/main/ig/StructureDefinition-BundleAgregateur.xlsx
+++ b/main/ig/StructureDefinition-BundleAgregateur.xlsx
@@ -54,7 +54,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2024-12-03T16:43:00+00:00</t>
+    <t>2024-12-03T17:24:51+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -78,7 +78,7 @@
     <t>Description</t>
   </si>
   <si>
-    <t>Profil de Bundle qui représente le flux de réponse contenant les créneaux disponibles dans le cadre du service d'agrégation de créneaux de la plateforme SAS (Service d'accès aux soins)</t>
+    <t>Profil de Bundle qui représente le flux de réponse contenant les créneaux disponibles dans le cadre du service d'agrégation de créneaux de la plateforme SAS - Cas d'usage PS Indiv</t>
   </si>
   <si>
     <t>Purpose</t>

</xml_diff>

<commit_message>
Validation release 1.1.0 (#94)
* Change files for release 1.1.0

* Change trial-use to trial-implementation

* Update release-notes.md 1927e3c2b00e053ee970f8d94e63d163fe3f27a2
</commit_message>
<xml_diff>
--- a/main/ig/StructureDefinition-BundleAgregateur.xlsx
+++ b/main/ig/StructureDefinition-BundleAgregateur.xlsx
@@ -30,7 +30,7 @@
     <t>Version</t>
   </si>
   <si>
-    <t>1.0.0</t>
+    <t>1.1.0</t>
   </si>
   <si>
     <t>Name</t>
@@ -54,7 +54,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2024-12-03T17:24:51+00:00</t>
+    <t>2024-12-05T15:50:46+00:00</t>
   </si>
   <si>
     <t>Publisher</t>

</xml_diff>

<commit_message>
Ajout date de création (#105)
MS sur date de création du RDV fa60d11f2d8f6e692015acce12568a136d01ed28
</commit_message>
<xml_diff>
--- a/main/ig/StructureDefinition-BundleAgregateur.xlsx
+++ b/main/ig/StructureDefinition-BundleAgregateur.xlsx
@@ -54,7 +54,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2025-03-12T14:15:42+00:00</t>
+    <t>2025-07-01T07:19:50+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -1649,17 +1649,17 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="74.20703125" customWidth="true" bestFit="true"/>
-    <col min="2" max="2" width="39.0078125" customWidth="true" bestFit="true"/>
-    <col min="3" max="3" width="35.625" customWidth="true" bestFit="true" hidden="true"/>
-    <col min="4" max="4" width="21.21875" customWidth="true" bestFit="true" hidden="true"/>
-    <col min="5" max="5" width="6.77734375" customWidth="true" bestFit="true"/>
-    <col min="6" max="6" width="4.9453125" customWidth="true" bestFit="true"/>
-    <col min="7" max="7" width="5.4296875" customWidth="true" bestFit="true"/>
-    <col min="8" max="8" width="16.27734375" customWidth="true" bestFit="true"/>
-    <col min="9" max="9" width="13.26171875" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" width="63.6171875" customWidth="true" bestFit="true"/>
+    <col min="2" max="2" width="33.44140625" customWidth="true" bestFit="true"/>
+    <col min="3" max="3" width="30.54296875" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="4" max="4" width="18.19140625" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="5" max="5" width="5.80859375" customWidth="true" bestFit="true"/>
+    <col min="6" max="6" width="4.23828125" customWidth="true" bestFit="true"/>
+    <col min="7" max="7" width="4.65625" customWidth="true" bestFit="true"/>
+    <col min="8" max="8" width="13.953125" customWidth="true" bestFit="true"/>
+    <col min="9" max="9" width="11.3671875" customWidth="true" bestFit="true"/>
     <col min="10" max="10" width="20.703125" customWidth="true" bestFit="true"/>
-    <col min="11" max="11" width="86.1875" customWidth="true" bestFit="true"/>
+    <col min="11" max="11" width="73.890625" customWidth="true" bestFit="true"/>
     <col min="12" max="12" width="100.703125" customWidth="true" bestFit="true"/>
     <col min="13" max="13" width="100.703125" customWidth="true" bestFit="true"/>
     <col min="14" max="14" width="100.703125" customWidth="true" bestFit="true"/>
@@ -1668,26 +1668,26 @@
     <col min="17" max="17" width="20.703125" customWidth="true" bestFit="true"/>
     <col min="18" max="18" width="20.703125" customWidth="true" bestFit="true"/>
     <col min="19" max="19" width="20.703125" customWidth="true" bestFit="true"/>
-    <col min="20" max="20" width="9.953125" customWidth="true" bestFit="true"/>
-    <col min="21" max="21" width="17.171875" customWidth="true" bestFit="true"/>
-    <col min="22" max="22" width="17.65625" customWidth="true" bestFit="true"/>
-    <col min="23" max="23" width="19.03515625" customWidth="true" bestFit="true"/>
-    <col min="24" max="24" width="18.859375" customWidth="true" bestFit="true"/>
-    <col min="25" max="25" width="168.19140625" customWidth="true" bestFit="true"/>
-    <col min="26" max="26" width="49.01171875" customWidth="true" bestFit="true"/>
-    <col min="27" max="27" width="6.34765625" customWidth="true" bestFit="true"/>
-    <col min="28" max="28" width="22.71875" customWidth="true" bestFit="true"/>
-    <col min="29" max="29" width="42.03515625" customWidth="true" bestFit="true"/>
-    <col min="30" max="30" width="17.21484375" customWidth="true" bestFit="true"/>
-    <col min="31" max="31" width="14.4140625" customWidth="true" bestFit="true" hidden="true"/>
-    <col min="32" max="32" width="34.98046875" customWidth="true" bestFit="true" hidden="true"/>
-    <col min="33" max="33" width="10.5546875" customWidth="true" bestFit="true" hidden="true"/>
-    <col min="34" max="34" width="11.0390625" customWidth="true" bestFit="true"/>
+    <col min="20" max="20" width="8.53515625" customWidth="true" bestFit="true"/>
+    <col min="21" max="21" width="14.72265625" customWidth="true" bestFit="true"/>
+    <col min="22" max="22" width="15.13671875" customWidth="true" bestFit="true"/>
+    <col min="23" max="23" width="16.3203125" customWidth="true" bestFit="true"/>
+    <col min="24" max="24" width="16.16796875" customWidth="true" bestFit="true"/>
+    <col min="25" max="25" width="144.1953125" customWidth="true" bestFit="true"/>
+    <col min="26" max="26" width="42.01953125" customWidth="true" bestFit="true"/>
+    <col min="27" max="27" width="5.44140625" customWidth="true" bestFit="true"/>
+    <col min="28" max="28" width="19.4765625" customWidth="true" bestFit="true"/>
+    <col min="29" max="29" width="36.0390625" customWidth="true" bestFit="true"/>
+    <col min="30" max="30" width="14.7578125" customWidth="true" bestFit="true"/>
+    <col min="31" max="31" width="12.359375" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="32" max="32" width="29.98828125" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="33" max="33" width="9.046875" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="34" max="34" width="9.46484375" customWidth="true" bestFit="true"/>
     <col min="35" max="35" width="100.703125" customWidth="true"/>
-    <col min="37" max="37" width="62.87890625" customWidth="true" bestFit="true"/>
-    <col min="38" max="38" width="143.74609375" customWidth="true" bestFit="true"/>
-    <col min="39" max="39" width="42.9765625" customWidth="true" bestFit="true"/>
-    <col min="40" max="40" width="36.91796875" customWidth="true" bestFit="true"/>
+    <col min="37" max="37" width="53.91015625" customWidth="true" bestFit="true"/>
+    <col min="38" max="38" width="123.23828125" customWidth="true" bestFit="true"/>
+    <col min="39" max="39" width="36.84375" customWidth="true" bestFit="true"/>
+    <col min="40" max="40" width="31.65234375" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -7859,7 +7859,7 @@
         <v>76</v>
       </c>
       <c r="J55" t="s" s="2">
-        <v>76</v>
+        <v>87</v>
       </c>
       <c r="K55" t="s" s="2">
         <v>281</v>
@@ -11497,7 +11497,7 @@
         <v>76</v>
       </c>
       <c r="J87" t="s" s="2">
-        <v>76</v>
+        <v>87</v>
       </c>
       <c r="K87" t="s" s="2">
         <v>318</v>
@@ -15135,7 +15135,7 @@
         <v>76</v>
       </c>
       <c r="J119" t="s" s="2">
-        <v>76</v>
+        <v>87</v>
       </c>
       <c r="K119" t="s" s="2">
         <v>354</v>
@@ -18773,7 +18773,7 @@
         <v>76</v>
       </c>
       <c r="J151" t="s" s="2">
-        <v>76</v>
+        <v>87</v>
       </c>
       <c r="K151" t="s" s="2">
         <v>392</v>

</xml_diff>